<commit_message>
Reestructura de la unidad de control y adición de mnemonicos
</commit_message>
<xml_diff>
--- a/COMPILADOR/mnemonicos.xlsx
+++ b/COMPILADOR/mnemonicos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\ARQUITECTURA DE MICROPROCESADORES\arquitectura-digital\COMPILADOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\ARQUITECTURA DE MICROCONTROLADORES Y MICROPROCESADORES\arquitectura-digital\COMPILADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B1ABB2-BB5C-4142-A989-9209FD8CD57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8574A3-FC0E-4C20-AEF1-A1F720CF997E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{B04DD6CF-0AF0-4ADE-AC0F-EE3CDD0CF55D}"/>
+    <workbookView xWindow="7188" yWindow="804" windowWidth="11508" windowHeight="11580" xr2:uid="{B04DD6CF-0AF0-4ADE-AC0F-EE3CDD0CF55D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Instrucción</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Obtener el valor de una dirección en el registro y dirigirlo a la salida A</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>Cargar el registro desde memoria</t>
   </si>
 </sst>
 </file>
@@ -525,19 +531,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42E7A41-1069-407C-ACD8-ABC73ADA16BF}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -559,7 +565,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -570,7 +576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -581,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -592,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -603,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -614,7 +620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -625,7 +631,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -636,7 +642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -647,7 +653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -658,7 +664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -669,7 +675,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -680,7 +686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -691,14 +697,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2">
         <v>1101</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1110</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>